<commit_message>
added data screenshots, checked data dictionary for typos
</commit_message>
<xml_diff>
--- a/docs/datadictionary.xlsx
+++ b/docs/datadictionary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC014556-B135-497B-9BE8-EF4F764E7C13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE50F654-1209-4596-B81D-39D501DF2F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Adopted Budgets</t>
   </si>
   <si>
-    <t>Filed Name</t>
-  </si>
-  <si>
     <t>Service Name</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>PerCapita</t>
   </si>
   <si>
-    <t>Tranc2</t>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
@@ -277,6 +271,12 @@
   </si>
   <si>
     <t>amount of the transaction</t>
+  </si>
+  <si>
+    <t>Field name</t>
+  </si>
+  <si>
+    <t>Trans2</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,19 +644,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,361 +664,361 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
         <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
         <v>76</v>
-      </c>
-      <c r="E24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
noted fields that could be removed in data dictionary
</commit_message>
<xml_diff>
--- a/docs/datadictionary.xlsx
+++ b/docs/datadictionary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE50F654-1209-4596-B81D-39D501DF2F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014DEB99-F331-47D3-9222-64233EF81B97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>Files</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Personnel expenses, property tax</t>
   </si>
   <si>
-    <t>should be unique</t>
-  </si>
-  <si>
     <t>"100001-41101"</t>
   </si>
   <si>
@@ -277,6 +274,15 @@
   </si>
   <si>
     <t>Trans2</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>AU x year unique</t>
+  </si>
+  <si>
+    <t>AU x year unique (AU = Service# - Acct#)</t>
   </si>
 </sst>
 </file>
@@ -625,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -725,6 +731,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -879,6 +888,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -886,16 +898,19 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -936,21 +951,24 @@
       <c r="F20" t="s">
         <v>28</v>
       </c>
+      <c r="G20" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
         <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -959,10 +977,10 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
         <v>77</v>
-      </c>
-      <c r="E23" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,10 +991,10 @@
         <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -987,10 +1005,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
@@ -1004,10 +1022,10 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
         <v>79</v>
-      </c>
-      <c r="E26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1015,10 +1033,10 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>